<commit_message>
22/09/2011 Thầy Tú cập nhật trạng thái công việc cập nhật dữ liệu vào csdl
</commit_message>
<xml_diff>
--- a/01. Documents/TRM Project v2011.09.10.xlsx
+++ b/01. Documents/TRM Project v2011.09.10.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Plan!$A$10:$BF$55</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -1088,7 +1088,7 @@
   <dimension ref="A2:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1285,10 +1285,10 @@
   <dimension ref="A1:BE55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="10" topLeftCell="E27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="10" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1897,7 +1897,7 @@
       <c r="BD10" s="22"/>
       <c r="BE10" s="22"/>
     </row>
-    <row r="11" spans="1:57" hidden="1">
+    <row r="11" spans="1:57">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1976,7 +1976,7 @@
       <c r="BD11" s="1"/>
       <c r="BE11" s="1"/>
     </row>
-    <row r="12" spans="1:57" hidden="1">
+    <row r="12" spans="1:57">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="BD13" s="1"/>
       <c r="BE13" s="1"/>
     </row>
-    <row r="14" spans="1:57">
+    <row r="14" spans="1:57" hidden="1">
       <c r="A14">
         <v>4</v>
       </c>
@@ -2276,7 +2276,7 @@
       <c r="BD15" s="22"/>
       <c r="BE15" s="22"/>
     </row>
-    <row r="16" spans="1:57" hidden="1">
+    <row r="16" spans="1:57">
       <c r="A16">
         <v>6</v>
       </c>
@@ -2351,7 +2351,7 @@
       <c r="BD16" s="1"/>
       <c r="BE16" s="1"/>
     </row>
-    <row r="17" spans="1:57" hidden="1">
+    <row r="17" spans="1:57">
       <c r="A17">
         <v>7</v>
       </c>
@@ -2426,7 +2426,7 @@
       <c r="BD17" s="1"/>
       <c r="BE17" s="1"/>
     </row>
-    <row r="18" spans="1:57" hidden="1">
+    <row r="18" spans="1:57">
       <c r="A18">
         <v>8</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>40805</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
@@ -2501,7 +2501,7 @@
       <c r="BD18" s="1"/>
       <c r="BE18" s="1"/>
     </row>
-    <row r="19" spans="1:57" hidden="1">
+    <row r="19" spans="1:57">
       <c r="A19">
         <v>9</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>40806</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I19" s="23"/>
       <c r="J19" s="23"/>
@@ -2576,7 +2576,7 @@
       <c r="BD19" s="1"/>
       <c r="BE19" s="1"/>
     </row>
-    <row r="20" spans="1:57" hidden="1">
+    <row r="20" spans="1:57">
       <c r="A20">
         <v>10</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>40807</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I20" s="23"/>
       <c r="J20" s="23"/>
@@ -2651,7 +2651,7 @@
       <c r="BD20" s="1"/>
       <c r="BE20" s="1"/>
     </row>
-    <row r="21" spans="1:57" hidden="1">
+    <row r="21" spans="1:57">
       <c r="A21">
         <v>11</v>
       </c>
@@ -2726,7 +2726,7 @@
       <c r="BD21" s="1"/>
       <c r="BE21" s="1"/>
     </row>
-    <row r="22" spans="1:57" hidden="1">
+    <row r="22" spans="1:57">
       <c r="A22">
         <v>12</v>
       </c>
@@ -3099,7 +3099,7 @@
       <c r="BD26" s="1"/>
       <c r="BE26" s="1"/>
     </row>
-    <row r="27" spans="1:57">
+    <row r="27" spans="1:57" hidden="1">
       <c r="A27">
         <v>17</v>
       </c>
@@ -3180,7 +3180,7 @@
       <c r="BD27" s="1"/>
       <c r="BE27" s="1"/>
     </row>
-    <row r="28" spans="1:57">
+    <row r="28" spans="1:57" hidden="1">
       <c r="A28">
         <v>18</v>
       </c>
@@ -3403,7 +3403,7 @@
       <c r="BD30" s="22"/>
       <c r="BE30" s="22"/>
     </row>
-    <row r="31" spans="1:57">
+    <row r="31" spans="1:57" hidden="1">
       <c r="A31">
         <v>21</v>
       </c>
@@ -3482,7 +3482,7 @@
       <c r="BD31" s="1"/>
       <c r="BE31" s="1"/>
     </row>
-    <row r="32" spans="1:57" ht="30">
+    <row r="32" spans="1:57" ht="30" hidden="1">
       <c r="A32">
         <v>22</v>
       </c>
@@ -3561,7 +3561,7 @@
       <c r="BD32" s="1"/>
       <c r="BE32" s="1"/>
     </row>
-    <row r="33" spans="1:57" ht="30">
+    <row r="33" spans="1:57" ht="30" hidden="1">
       <c r="A33">
         <v>23</v>
       </c>
@@ -3640,7 +3640,7 @@
       <c r="BD33" s="1"/>
       <c r="BE33" s="1"/>
     </row>
-    <row r="34" spans="1:57" ht="30">
+    <row r="34" spans="1:57" ht="30" hidden="1">
       <c r="A34">
         <v>24</v>
       </c>
@@ -3889,7 +3889,7 @@
       <c r="BD36" s="1"/>
       <c r="BE36" s="1"/>
     </row>
-    <row r="37" spans="1:57" ht="30">
+    <row r="37" spans="1:57" ht="30" hidden="1">
       <c r="A37">
         <v>27</v>
       </c>
@@ -3970,7 +3970,7 @@
       <c r="BD37" s="1"/>
       <c r="BE37" s="1"/>
     </row>
-    <row r="38" spans="1:57">
+    <row r="38" spans="1:57" hidden="1">
       <c r="A38">
         <v>28</v>
       </c>
@@ -4552,7 +4552,7 @@
       <c r="BD45" s="1"/>
       <c r="BE45" s="1"/>
     </row>
-    <row r="46" spans="1:57" hidden="1">
+    <row r="46" spans="1:57">
       <c r="A46">
         <v>36</v>
       </c>
@@ -5211,8 +5211,8 @@
   </sheetData>
   <autoFilter ref="A10:BF55">
     <filterColumn colId="3">
-      <filters blank="1">
-        <filter val="LinhDH"/>
+      <filters>
+        <filter val="Tund"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>